<commit_message>
MOD:Changes in process description for Activos2
</commit_message>
<xml_diff>
--- a/cl.bancochile.fdd.master.cmf/src/resources/pd/PD_tbl_cmf_Activos2_mes.xlsx
+++ b/cl.bancochile.fdd.master.cmf/src/resources/pd/PD_tbl_cmf_Activos2_mes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1220212.SOAM\Desktop\PreSales\Banco de Chile\2020-11-28 - Gobierno de Datos - Monovendor Células Ágiles Datalake\FDs and PDs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7720828F-69D7-45FD-A747-AA00E65B4F34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A585B400-F812-4216-B4B0-49E62FDEF6FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Format Details" sheetId="1" r:id="rId1"/>
+    <sheet name="DQ Validaciones" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>Institucion</t>
   </si>
@@ -222,13 +223,52 @@
   </si>
   <si>
     <t>Total de activos de consumo</t>
+  </si>
+  <si>
+    <t>Validations</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Activos Bancos 2</t>
+  </si>
+  <si>
+    <t>column Z = column C + G + L</t>
+  </si>
+  <si>
+    <t>column L = column N + P</t>
+  </si>
+  <si>
+    <t>column C = column D + E</t>
+  </si>
+  <si>
+    <t>column G = column H + I</t>
+  </si>
+  <si>
+    <t>column B = column C + G + K - F - J</t>
+  </si>
+  <si>
+    <t>column L = column N + S + T + U + W</t>
+  </si>
+  <si>
+    <t>Activos Bancos 1 cross Activos Bancos 2</t>
+  </si>
+  <si>
+    <t>activos1 . Column B = activos 2 . Column Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column Z  
+    minimum value 0 
+    maximum value 100.000.000
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,8 +288,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +314,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -350,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -371,6 +423,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,4 +1061,95 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE453B23-573A-4E9A-9BB0-5455D074E784}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>